<commit_message>
commiting test classes (#3)
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\DSAlgo.RockStars\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7681349B-65EB-44AD-8DFE-5931AB71D109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="2" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="dsalgocode" sheetId="3" r:id="rId3"/>
+    <sheet name="registerpage" sheetId="4" r:id="rId4"/>
+    <sheet name="logindata" sheetId="5" r:id="rId5"/>
+    <sheet name="validcode" sheetId="6" r:id="rId6"/>
+    <sheet name="invalidcode" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
   <si>
     <t>output</t>
   </si>
@@ -169,12 +167,94 @@
 \b
 search([12, 23, 45, 67, 6, 90] , 12)</t>
   </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>passwordconfirmation</t>
+  </si>
+  <si>
+    <t>errormsg</t>
+  </si>
+  <si>
+    <t>Lillyy_1@991</t>
+  </si>
+  <si>
+    <t>testPassword@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testPassword@1 </t>
+  </si>
+  <si>
+    <t>username already exists</t>
+  </si>
+  <si>
+    <t>Raha_a@123</t>
+  </si>
+  <si>
+    <t>ah_1@4</t>
+  </si>
+  <si>
+    <t>aha_1@456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter a valid username </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password cannot be only numeric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aha_1@4567 </t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Password should be atleast </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> characters </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&amp;&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008080"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**&amp;&amp;**</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,16 +276,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -276,10 +407,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -289,11 +424,28 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -352,7 +504,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -404,7 +556,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -598,27 +750,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76ECF3AC-3B24-42EA-9B15-33AE01380818}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="88.6328125" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -626,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,13 +786,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -648,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -656,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -664,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -672,7 +824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -680,7 +832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -688,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -696,7 +848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -710,72 +862,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181E224E-2837-0142-8AD8-569527ABC061}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6328125" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="18.5">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" ht="18.5">
+      <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" ht="18.5">
+      <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:3" ht="18.5">
+      <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" ht="18.5">
+      <c r="A5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -785,28 +937,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9429FDAC-9F73-44C8-B623-9BE65DFF2AC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="195.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -814,13 +966,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -828,7 +980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -836,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -844,7 +996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -852,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -860,7 +1012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -868,7 +1020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -876,12 +1028,220 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16.1796875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="57.81640625" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="15.5">
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="10" customFormat="1" ht="15.5">
+      <c r="A2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="10" customFormat="1" ht="15.5">
+      <c r="A3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="10" customFormat="1" ht="15.5">
+      <c r="A4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="10" customFormat="1" ht="15.5">
+      <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="14">
+        <v>12345678</v>
+      </c>
+      <c r="C5" s="14">
+        <v>12345678</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="10" customFormat="1" ht="15.5">
+      <c r="A6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="C3" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId8"/>
+    <hyperlink ref="A2" r:id="rId9"/>
+    <hyperlink ref="A3" r:id="rId10"/>
+    <hyperlink ref="A5" r:id="rId11"/>
+    <hyperlink ref="A6" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5">
+      <c r="A2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting page classes and tast case page
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\DSAlgo.RockStars\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\Dsalgo.Testngframeworks\Dsalgo.Testngframeworks\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7681349B-65EB-44AD-8DFE-5931AB71D109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F180335F-1986-4C17-B1A6-51FE34A45F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="2" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="3" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="dsalgocode" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
   <si>
     <t>output</t>
   </si>
@@ -168,6 +169,15 @@
 \b
 \b
 search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Some Tests failed. Please review code</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No tests were collected</t>
   </si>
 </sst>
 </file>
@@ -786,10 +796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9429FDAC-9F73-44C8-B623-9BE65DFF2AC9}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,6 +808,108 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F02A834-137D-4814-B962-82A643003AFD}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>12</v>
@@ -832,8 +944,8 @@
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -848,8 +960,8 @@
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
+      <c r="B7" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -864,8 +976,8 @@
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>6</v>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -880,8 +992,8 @@
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>6</v>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing QueueTest.java, RegisterTest.java,Utils.java,excel sheet,DataProviderClass.java
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\Dsalgo.Testngframeworks\Dsalgo.Testngframeworks\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F180335F-1986-4C17-B1A6-51FE34A45F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="3" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="dsalgocode" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="registerpage" sheetId="5" r:id="rId5"/>
+    <sheet name="logindata" sheetId="6" r:id="rId6"/>
+    <sheet name="validcode" sheetId="7" r:id="rId7"/>
+    <sheet name="invalidcode" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>output</t>
   </si>
@@ -179,12 +177,91 @@
   <si>
     <t xml:space="preserve"> No tests were collected</t>
   </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>passwordconfirmation</t>
+  </si>
+  <si>
+    <t>errormsg</t>
+  </si>
+  <si>
+    <t>Lillyy_1@991</t>
+  </si>
+  <si>
+    <t>testPassword@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testPassword@1 </t>
+  </si>
+  <si>
+    <t>username already exists</t>
+  </si>
+  <si>
+    <t>Raha_a@123</t>
+  </si>
+  <si>
+    <t>ah_1@4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Password should be atleast </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> characters </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&amp;&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**&amp;&amp;**</t>
+    </r>
+  </si>
+  <si>
+    <t>aha_1@456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter a valid username </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password cannot be only numeric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aha_1@4567 </t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +293,37 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -286,10 +394,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -302,8 +414,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,7 +488,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -414,7 +540,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -608,27 +734,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76ECF3AC-3B24-42EA-9B15-33AE01380818}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="88.6328125" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -636,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,13 +770,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -658,7 +784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -666,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -674,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -682,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -690,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -698,7 +824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -706,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -720,21 +846,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181E224E-2837-0142-8AD8-569527ABC061}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="17.5">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -745,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="17.5">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -756,7 +882,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="17.5">
       <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
@@ -767,7 +893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="17.5">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -778,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="17.5">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
@@ -795,20 +921,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9429FDAC-9F73-44C8-B623-9BE65DFF2AC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="195.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -816,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -824,14 +950,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -839,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -847,7 +973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -855,7 +981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -863,7 +989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -871,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -879,7 +1005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -887,7 +1013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -901,16 +1027,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F02A834-137D-4814-B962-82A643003AFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -918,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -926,13 +1052,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -940,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -948,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -956,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -964,7 +1090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -972,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -980,7 +1106,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -988,12 +1114,226 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.5">
+      <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.5">
+      <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5">
+      <c r="A4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5">
+      <c r="A5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="C5" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="C3" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId8"/>
+    <hyperlink ref="A2" r:id="rId9"/>
+    <hyperlink ref="A3" r:id="rId10"/>
+    <hyperlink ref="A5" r:id="rId11"/>
+    <hyperlink ref="A6" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5">
+      <c r="A2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing QueueTest.java, RegisterTest.java,Utils.java,excel sheet,DataProviderClass.java (#8)
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\Dsalgo.Testngframeworks\Dsalgo.Testngframeworks\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F180335F-1986-4C17-B1A6-51FE34A45F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="3" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
     <sheet name="dsalgocode" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="registerpage" sheetId="5" r:id="rId5"/>
+    <sheet name="logindata" sheetId="6" r:id="rId6"/>
+    <sheet name="validcode" sheetId="7" r:id="rId7"/>
+    <sheet name="invalidcode" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>output</t>
   </si>
@@ -179,12 +177,91 @@
   <si>
     <t xml:space="preserve"> No tests were collected</t>
   </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>passwordconfirmation</t>
+  </si>
+  <si>
+    <t>errormsg</t>
+  </si>
+  <si>
+    <t>Lillyy_1@991</t>
+  </si>
+  <si>
+    <t>testPassword@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testPassword@1 </t>
+  </si>
+  <si>
+    <t>username already exists</t>
+  </si>
+  <si>
+    <t>Raha_a@123</t>
+  </si>
+  <si>
+    <t>ah_1@4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Password should be atleast </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> characters </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&amp;&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF008080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>**&amp;&amp;**</t>
+    </r>
+  </si>
+  <si>
+    <t>aha_1@456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter a valid username </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password cannot be only numeric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aha_1@4567 </t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +293,37 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -286,10 +394,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -302,8 +414,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,7 +488,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -414,7 +540,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -608,27 +734,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76ECF3AC-3B24-42EA-9B15-33AE01380818}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="88.6328125" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -636,7 +762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -644,13 +770,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -658,7 +784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -666,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -674,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -682,7 +808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -690,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -698,7 +824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -706,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -720,21 +846,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{181E224E-2837-0142-8AD8-569527ABC061}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="17.5">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -745,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="17.5">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
@@ -756,7 +882,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="17.5">
       <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
@@ -767,7 +893,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="17.5">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -778,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="17.5">
       <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
@@ -795,20 +921,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9429FDAC-9F73-44C8-B623-9BE65DFF2AC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="195.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -816,7 +942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -824,14 +950,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -839,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -847,7 +973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -855,7 +981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -863,7 +989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -871,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -879,7 +1005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -887,7 +1013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -901,16 +1027,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F02A834-137D-4814-B962-82A643003AFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -918,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -926,13 +1052,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -940,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -948,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -956,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -964,7 +1090,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -972,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -980,7 +1106,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -988,12 +1114,226 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.5">
+      <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.5">
+      <c r="A3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5">
+      <c r="A4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5">
+      <c r="A5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="C5" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
+    <hyperlink ref="C3" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId8"/>
+    <hyperlink ref="A2" r:id="rId9"/>
+    <hyperlink ref="A3" r:id="rId10"/>
+    <hyperlink ref="A5" r:id="rId11"/>
+    <hyperlink ref="A6" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5">
+      <c r="A2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login, DataStructure, Stack, Graph
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnaveniram/git/Dsalgo.Testngframework/Dsalgo.Testngframeworks/src/test/resources/TestData/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2EF709-BBD3-A84A-ABD0-E08422B4E7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="7"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="22540" windowHeight="14300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
@@ -17,8 +23,8 @@
     <sheet name="invalidcode" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
   <si>
     <t>output</t>
   </si>
@@ -119,31 +125,16 @@
     <t>pythonCode</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Expected Message</t>
   </si>
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>sdet84batch</t>
-  </si>
-  <si>
     <t>Invalid Username and Password</t>
   </si>
   <si>
     <t>Rockstars_Numpy</t>
-  </si>
-  <si>
-    <t>sdet86batch</t>
-  </si>
-  <si>
-    <t>Numpysdet86</t>
   </si>
   <si>
     <t>Numpy@Rock123</t>
@@ -256,12 +247,24 @@
   <si>
     <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>sdet84batch</t>
+  </si>
+  <si>
+    <t>NameError: name 'Hello' is not defined on line 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,12 +284,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -324,6 +321,12 @@
       <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -396,12 +399,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -412,20 +415,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -488,7 +492,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -540,7 +544,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -734,27 +738,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="88.6328125" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="88.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -762,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -770,13 +774,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -784,7 +788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -792,7 +796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -800,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -808,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -816,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -824,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -832,7 +836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -846,73 +850,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.5">
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.5">
-      <c r="A3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.5">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.5">
-      <c r="A5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>23</v>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -921,59 +939,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="195.1796875" customWidth="1"/>
+    <col min="1" max="1" width="195.1640625" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -981,15 +999,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -997,7 +1015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1005,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1013,7 +1031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1027,54 +1045,54 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1082,15 +1100,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1098,15 +1116,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1114,12 +1132,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1128,152 +1146,152 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.5">
-      <c r="A2" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5">
-      <c r="A3" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="10" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="C5" s="11">
+        <v>12345678</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="11" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5">
-      <c r="A4" s="11" t="s">
+      <c r="D6" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5">
-      <c r="A5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="12">
-        <v>12345678</v>
-      </c>
-      <c r="C5" s="12">
-        <v>12345678</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B3" r:id="rId5"/>
-    <hyperlink ref="C2" r:id="rId6"/>
-    <hyperlink ref="C3" r:id="rId7"/>
-    <hyperlink ref="B2" r:id="rId8"/>
-    <hyperlink ref="A2" r:id="rId9"/>
-    <hyperlink ref="A3" r:id="rId10"/>
-    <hyperlink ref="A5" r:id="rId11"/>
-    <hyperlink ref="A6" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="B2" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="A2" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="A3" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="A5" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="A6" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.5">
-      <c r="A2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1282,20 +1300,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1303,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1317,23 +1335,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting extent reports, logs, listeners and crossbrowser xml
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="7"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="logindata" sheetId="6" r:id="rId6"/>
     <sheet name="validcode" sheetId="7" r:id="rId7"/>
     <sheet name="invalidcode" sheetId="8" r:id="rId8"/>
+    <sheet name="tryeditorcode" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>output</t>
   </si>
@@ -734,7 +735,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1320,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1339,4 +1340,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commiting extent reports, logs, listeners and crossbrowser xml (#15)
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="7"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="logindata" sheetId="6" r:id="rId6"/>
     <sheet name="validcode" sheetId="7" r:id="rId7"/>
     <sheet name="invalidcode" sheetId="8" r:id="rId8"/>
+    <sheet name="tryeditorcode" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>output</t>
   </si>
@@ -734,7 +735,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1320,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1339,4 +1340,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pushing new excel sheet
</commit_message>
<xml_diff>
--- a/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/Dsalgo.Testngframeworks/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siris\git\Dsalgo.Testngframeworks\Dsalgo.Testngframeworks\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDEF138-23F7-4A44-BC73-2FFA6CFF122F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" activeTab="7"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="python code" sheetId="1" r:id="rId1"/>
@@ -15,10 +21,12 @@
     <sheet name="logindata" sheetId="6" r:id="rId6"/>
     <sheet name="validcode" sheetId="7" r:id="rId7"/>
     <sheet name="invalidcode" sheetId="8" r:id="rId8"/>
+    <sheet name="Invalidcodeveni" sheetId="9" r:id="rId9"/>
+    <sheet name="tryeditorcode" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
   <si>
     <t>output</t>
   </si>
@@ -119,12 +127,6 @@
     <t>pythonCode</t>
   </si>
   <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Expected Message</t>
   </si>
   <si>
@@ -138,12 +140,6 @@
   </si>
   <si>
     <t>Rockstars_Numpy</t>
-  </si>
-  <si>
-    <t>sdet86batch</t>
-  </si>
-  <si>
-    <t>Numpysdet86</t>
   </si>
   <si>
     <t>Numpy@Rock123</t>
@@ -256,12 +252,21 @@
   <si>
     <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
+  <si>
+    <t>NameError: name 'hello' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,7 +493,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -540,7 +545,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -734,27 +739,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="88.6328125" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -762,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -770,13 +775,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -784,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -792,7 +797,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -800,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -808,7 +813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -816,7 +821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -824,7 +829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -832,12 +837,48 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96BDC24-C219-46A2-AD8D-BFBD3B7B5A03}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -846,73 +887,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5">
+    <row r="1" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.5">
-      <c r="A2" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.5">
-      <c r="A3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17.5">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.5">
-      <c r="A5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -921,20 +976,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="195.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -942,38 +997,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -981,15 +1036,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -997,7 +1052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1005,7 +1060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1013,7 +1068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1027,16 +1082,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
@@ -1044,37 +1099,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1082,15 +1137,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1098,15 +1153,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1114,12 +1169,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1128,14 +1183,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
@@ -1143,65 +1198,65 @@
     <col min="4" max="4" width="51.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5">
-      <c r="A2" s="10" t="s">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="11" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.5">
-      <c r="A3" s="10" t="s">
+      <c r="B4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5">
-      <c r="A4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5">
+    </row>
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="12">
         <v>12345678</v>
@@ -1210,92 +1265,92 @@
         <v>12345678</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B3" r:id="rId5"/>
-    <hyperlink ref="C2" r:id="rId6"/>
-    <hyperlink ref="C3" r:id="rId7"/>
-    <hyperlink ref="B2" r:id="rId8"/>
-    <hyperlink ref="A2" r:id="rId9"/>
-    <hyperlink ref="A3" r:id="rId10"/>
-    <hyperlink ref="A5" r:id="rId11"/>
-    <hyperlink ref="A6" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="B2" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="A2" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="A3" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="A5" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="A6" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.5">
-      <c r="A2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1303,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1317,23 +1372,57 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2DA217-0AEB-476D-9D90-94BF9AE909CF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>